<commit_message>
CCS for NMM fix + checking Ind PAMS work
Checking PAMS works in new model setup for Industry. fixing bits and adding lever switches for PAMS. 
Created new energy transmission techs for cement and lime so combustion emissions are included in CCS there.
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_IND/PP_constraints.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_IND/PP_constraints.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\TCH_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D96140-C4F9-407A-9F69-995402C27CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC9D41A-85B3-4B13-8A4A-840DF547F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E9085F61-4CF2-4A17-84B6-F025775E748A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9085F61-4CF2-4A17-84B6-F025775E748A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="index" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$AO$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$AO$45</definedName>
     <definedName name="impswitch_pp">[1]Index!$E$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="66">
   <si>
     <t>REGION1</t>
   </si>
@@ -237,6 +238,12 @@
   <si>
     <t>*</t>
   </si>
+  <si>
+    <t>ITEMS</t>
+  </si>
+  <si>
+    <t>Import constraints to model?</t>
+  </si>
 </sst>
 </file>
 
@@ -382,9 +389,9 @@
       <sheetName val="2012 SATIM EB"/>
       <sheetName val="2017 SATIM EB"/>
       <sheetName val="IND old - 2006BY"/>
+      <sheetName val="IND"/>
       <sheetName val="IND2017"/>
-      <sheetName val="IND"/>
-      <sheetName val="PAMS"/>
+      <sheetName val="PAMS central control panel"/>
       <sheetName val="ITEMS_Tech"/>
       <sheetName val="ITEMS_Comm"/>
       <sheetName val="TS DTech"/>
@@ -477,13 +484,7 @@
       <sheetData sheetId="55"/>
       <sheetData sheetId="56"/>
       <sheetData sheetId="57"/>
-      <sheetData sheetId="58">
-        <row r="18">
-          <cell r="M18">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="58"/>
       <sheetData sheetId="59"/>
       <sheetData sheetId="60"/>
       <sheetData sheetId="61"/>
@@ -524,6 +525,7 @@
       <sheetName val="ANSv2-692-Home"/>
       <sheetName val="Index"/>
       <sheetName val="PAMS levers"/>
+      <sheetName val="Students reprot"/>
       <sheetName val="RES"/>
       <sheetName val="EB_Exist"/>
       <sheetName val="ANSv2-692-REGIONS"/>
@@ -537,8 +539,8 @@
       <sheetName val="ANSv2-692-ProcData"/>
       <sheetName val="ProcData_plants and boilers"/>
       <sheetName val="ProcData_CHP"/>
+      <sheetName val="links to constraints"/>
       <sheetName val="ProcData_Xtechs"/>
-      <sheetName val="links to constraints"/>
       <sheetName val="Capital costs"/>
       <sheetName val="ANSv2-692-ConstrData"/>
       <sheetName val="ANSv2-692-ITEMS"/>
@@ -575,9 +577,14 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18">
+        <row r="1">
+          <cell r="C1" t="b">
+            <v>0</v>
+          </cell>
+        </row>
         <row r="4">
           <cell r="C4">
-            <v>1.6224025174380639</v>
+            <v>1.0643442529852023</v>
           </cell>
         </row>
         <row r="5">
@@ -587,7 +594,7 @@
         </row>
         <row r="6">
           <cell r="C6">
-            <v>0.44845060979707235</v>
+            <v>0.2941969234853859</v>
           </cell>
         </row>
         <row r="7">
@@ -597,12 +604,12 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>0.4152051071791632</v>
+            <v>1.719529411764706</v>
           </cell>
         </row>
         <row r="13">
           <cell r="C13">
-            <v>0.08</v>
+            <v>-0.16</v>
           </cell>
         </row>
       </sheetData>
@@ -615,6 +622,7 @@
       <sheetData sheetId="25"/>
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -916,12 +924,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FDDD9F-2C3B-406C-A725-1972B126B5CE}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="b">
+        <f>'[2]links to constraints'!$C$1</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655089F-1CBB-471E-94C2-BED83A3F5E8D}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,9 +966,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="str">
-        <f>IF(impswitch_pp,IF([1]IND!M18,"","ITEMS"),"")</f>
-        <v>ITEMS</v>
+      <c r="A1" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -947,7 +978,10 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -965,7 +999,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -983,7 +1020,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1001,7 +1041,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1062,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1037,7 +1083,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1055,7 +1104,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1073,7 +1125,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1091,7 +1146,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1109,7 +1167,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1127,7 +1188,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1145,7 +1209,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1163,7 +1230,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1181,7 +1251,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1199,7 +1272,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1293,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1242,13 +1321,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:AO45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1339,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1306,7 +1385,7 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1415,7 +1494,11 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1442,134 +1525,138 @@
       </c>
       <c r="J3" s="3">
         <f>'[2]links to constraints'!$C$4</f>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="K3" s="4">
         <f>J3</f>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="L3" s="4">
         <f t="shared" ref="L3:AO3" si="0">K3</f>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="Q3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="R3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="T3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="U3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="V3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="W3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="X3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="Y3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="Z3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AA3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AB3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AC3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AD3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AE3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AF3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AH3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AI3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AJ3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AK3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AL3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AM3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AN3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AO3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+        <v>1.0643442529852023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1691,7 +1778,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1813,7 +1904,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
@@ -1838,7 +1933,7 @@
       <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <f>'[2]links to constraints'!$C$5</f>
         <v>0.9305042796234908</v>
       </c>
@@ -1967,7 +2062,11 @@
         <v>0.9305042796234908</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2089,7 +2188,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
@@ -2211,7 +2314,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
@@ -2238,134 +2345,138 @@
       </c>
       <c r="J9" s="3">
         <f>'[2]links to constraints'!$C$6</f>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="K9" s="4">
         <f>J9</f>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" ref="L9:AO9" si="2">K9</f>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="O9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="S9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="T9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="U9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="V9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="W9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="X9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="Y9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="Z9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AA9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AB9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AC9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AD9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AE9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AF9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AH9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AI9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AJ9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AK9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AL9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AM9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AN9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AO9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+        <v>0.2941969234853859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -2487,7 +2598,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
@@ -2609,7 +2724,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
@@ -2634,7 +2753,7 @@
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="3">
         <f>'[2]links to constraints'!$C$7</f>
         <v>3.0777317647058822</v>
       </c>
@@ -2763,7 +2882,11 @@
         <v>3.0777317647058822</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2885,7 +3008,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
@@ -3007,7 +3134,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
@@ -3032,136 +3163,140 @@
       <c r="I15" s="1">
         <v>0</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="3">
         <f>'[2]links to constraints'!$C$8</f>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="K15" s="4">
         <f>J15</f>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" ref="L15:AO15" si="4">K15</f>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="S15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="T15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="U15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="V15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="W15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="X15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="Y15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="Z15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AA15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AB15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AC15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AD15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AE15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AF15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AG15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AH15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AI15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AJ15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AK15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AL15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AM15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AN15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AO15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
@@ -3283,7 +3418,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
@@ -3405,7 +3544,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -3527,7 +3670,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
@@ -3579,7 +3726,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="5">
         <f>-'[2]links to constraints'!$C$13</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
@@ -3587,7 +3734,7 @@
       <c r="AF19" s="2"/>
       <c r="AG19" s="2">
         <f>AB19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
@@ -3595,19 +3742,23 @@
       <c r="AK19" s="2"/>
       <c r="AL19" s="2">
         <f>AG19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2">
         <f>AL19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO19" s="2">
         <f>AN19</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
@@ -3729,7 +3880,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>39</v>
       </c>
@@ -3791,7 +3946,11 @@
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
     </row>
-    <row r="22" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
@@ -3913,7 +4072,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>39</v>
       </c>
@@ -3965,7 +4128,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2">
         <f>AB19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
@@ -3973,7 +4136,7 @@
       <c r="AF23" s="2"/>
       <c r="AG23" s="2">
         <f>AG19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
@@ -3981,19 +4144,23 @@
       <c r="AK23" s="2"/>
       <c r="AL23" s="2">
         <f>AL19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2">
         <f>AN19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO23" s="2">
         <f>AO19</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="24" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>39</v>
       </c>
@@ -4115,7 +4282,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
@@ -4177,7 +4348,11 @@
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
     </row>
-    <row r="26" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
@@ -4299,7 +4474,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
@@ -4351,7 +4530,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2">
         <f>AB23</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
@@ -4359,7 +4538,7 @@
       <c r="AF27" s="2"/>
       <c r="AG27" s="2">
         <f>AG23</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
@@ -4367,19 +4546,23 @@
       <c r="AK27" s="2"/>
       <c r="AL27" s="2">
         <f>AL23</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2">
         <f>AN23</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO27" s="2">
         <f>AO23</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="28" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
@@ -4501,7 +4684,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
@@ -4561,7 +4748,11 @@
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
     </row>
-    <row r="30" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
@@ -4683,7 +4874,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
@@ -4735,7 +4930,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2">
         <f>AB27</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
@@ -4743,7 +4938,7 @@
       <c r="AF31" s="2"/>
       <c r="AG31" s="2">
         <f>AG27</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
@@ -4751,19 +4946,23 @@
       <c r="AK31" s="2"/>
       <c r="AL31" s="2">
         <f>AL27</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2">
         <f>AN27</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO31" s="2">
         <f>AO27</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="32" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
@@ -4885,7 +5084,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B33" s="1" t="s">
         <v>39</v>
       </c>
@@ -4947,7 +5150,11 @@
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
     </row>
-    <row r="34" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
@@ -5069,7 +5276,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
@@ -5191,7 +5402,11 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="36" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
@@ -5313,7 +5528,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
@@ -5365,7 +5584,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2">
         <f>AB31</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -5373,7 +5592,7 @@
       <c r="AF37" s="2"/>
       <c r="AG37" s="2">
         <f>AG31</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
@@ -5381,19 +5600,23 @@
       <c r="AK37" s="2"/>
       <c r="AL37" s="2">
         <f>AL31</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM37" s="2"/>
       <c r="AN37" s="2">
         <f>AN31</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO37" s="2">
         <f>AO31</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="38" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B38" s="1" t="s">
         <v>39</v>
       </c>
@@ -5515,7 +5738,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
@@ -5575,7 +5802,11 @@
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
     </row>
-    <row r="40" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
@@ -5697,7 +5928,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B41" s="1" t="s">
         <v>59</v>
       </c>
@@ -5819,7 +6054,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B42" s="1" t="s">
         <v>59</v>
       </c>
@@ -5941,7 +6180,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B43" s="1" t="s">
         <v>59</v>
       </c>
@@ -6063,7 +6306,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B44" s="1" t="s">
         <v>59</v>
       </c>
@@ -6185,7 +6432,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B45" s="1" t="s">
         <v>59</v>
       </c>
@@ -6308,18 +6559,24 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO45" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}"/>
+  <autoFilter ref="A1:AO45" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="UC-IPPREC-MAX"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F99B7C9-5FBB-4C6F-BCA2-7100EC51A245}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6329,7 +6586,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" t="s">
@@ -6337,6 +6594,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
@@ -6363,6 +6624,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>61</v>
       </c>
@@ -6389,6 +6654,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>61</v>
       </c>
@@ -6415,6 +6684,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
@@ -6441,6 +6714,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
       </c>
@@ -6467,6 +6744,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>61</v>
       </c>
@@ -6493,6 +6774,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>61</v>
       </c>
@@ -6519,6 +6804,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
@@ -6545,6 +6834,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
@@ -6571,6 +6864,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>61</v>
       </c>
@@ -6597,6 +6894,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>61</v>
       </c>
@@ -6623,6 +6924,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>61</v>
       </c>
@@ -6649,6 +6954,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>61</v>
       </c>
@@ -6675,6 +6984,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>61</v>
       </c>
@@ -6701,6 +7014,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>61</v>
       </c>
@@ -6726,7 +7043,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Merge with Bryce's changes in Industry and a few other small fixes
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_IND/PP_constraints.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_IND/PP_constraints.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\TCH_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D96140-C4F9-407A-9F69-995402C27CDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC9D41A-85B3-4B13-8A4A-840DF547F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E9085F61-4CF2-4A17-84B6-F025775E748A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9085F61-4CF2-4A17-84B6-F025775E748A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="index" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId4"/>
     <externalReference r:id="rId5"/>
+    <externalReference r:id="rId6"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$AO$45</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Sheet2!$A$1:$AO$45</definedName>
     <definedName name="impswitch_pp">[1]Index!$E$21</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="66">
   <si>
     <t>REGION1</t>
   </si>
@@ -237,6 +238,12 @@
   <si>
     <t>*</t>
   </si>
+  <si>
+    <t>ITEMS</t>
+  </si>
+  <si>
+    <t>Import constraints to model?</t>
+  </si>
 </sst>
 </file>
 
@@ -382,9 +389,9 @@
       <sheetName val="2012 SATIM EB"/>
       <sheetName val="2017 SATIM EB"/>
       <sheetName val="IND old - 2006BY"/>
+      <sheetName val="IND"/>
       <sheetName val="IND2017"/>
-      <sheetName val="IND"/>
-      <sheetName val="PAMS"/>
+      <sheetName val="PAMS central control panel"/>
       <sheetName val="ITEMS_Tech"/>
       <sheetName val="ITEMS_Comm"/>
       <sheetName val="TS DTech"/>
@@ -477,13 +484,7 @@
       <sheetData sheetId="55"/>
       <sheetData sheetId="56"/>
       <sheetData sheetId="57"/>
-      <sheetData sheetId="58">
-        <row r="18">
-          <cell r="M18">
-            <v>0</v>
-          </cell>
-        </row>
-      </sheetData>
+      <sheetData sheetId="58"/>
       <sheetData sheetId="59"/>
       <sheetData sheetId="60"/>
       <sheetData sheetId="61"/>
@@ -524,6 +525,7 @@
       <sheetName val="ANSv2-692-Home"/>
       <sheetName val="Index"/>
       <sheetName val="PAMS levers"/>
+      <sheetName val="Students reprot"/>
       <sheetName val="RES"/>
       <sheetName val="EB_Exist"/>
       <sheetName val="ANSv2-692-REGIONS"/>
@@ -537,8 +539,8 @@
       <sheetName val="ANSv2-692-ProcData"/>
       <sheetName val="ProcData_plants and boilers"/>
       <sheetName val="ProcData_CHP"/>
+      <sheetName val="links to constraints"/>
       <sheetName val="ProcData_Xtechs"/>
-      <sheetName val="links to constraints"/>
       <sheetName val="Capital costs"/>
       <sheetName val="ANSv2-692-ConstrData"/>
       <sheetName val="ANSv2-692-ITEMS"/>
@@ -575,9 +577,14 @@
       <sheetData sheetId="16"/>
       <sheetData sheetId="17"/>
       <sheetData sheetId="18">
+        <row r="1">
+          <cell r="C1" t="b">
+            <v>0</v>
+          </cell>
+        </row>
         <row r="4">
           <cell r="C4">
-            <v>1.6224025174380639</v>
+            <v>1.0643442529852023</v>
           </cell>
         </row>
         <row r="5">
@@ -587,7 +594,7 @@
         </row>
         <row r="6">
           <cell r="C6">
-            <v>0.44845060979707235</v>
+            <v>0.2941969234853859</v>
           </cell>
         </row>
         <row r="7">
@@ -597,12 +604,12 @@
         </row>
         <row r="8">
           <cell r="C8">
-            <v>0.4152051071791632</v>
+            <v>1.719529411764706</v>
           </cell>
         </row>
         <row r="13">
           <cell r="C13">
-            <v>0.08</v>
+            <v>-0.16</v>
           </cell>
         </row>
       </sheetData>
@@ -615,6 +622,7 @@
       <sheetData sheetId="25"/>
       <sheetData sheetId="26"/>
       <sheetData sheetId="27"/>
+      <sheetData sheetId="28"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -916,12 +924,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FDDD9F-2C3B-406C-A725-1972B126B5CE}">
+  <dimension ref="B2:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" t="b">
+        <f>'[2]links to constraints'!$C$1</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F655089F-1CBB-471E-94C2-BED83A3F5E8D}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -934,9 +966,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="str">
-        <f>IF(impswitch_pp,IF([1]IND!M18,"","ITEMS"),"")</f>
-        <v>ITEMS</v>
+      <c r="A1" s="1" t="s">
+        <v>64</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -947,7 +978,10 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
+      <c r="A2" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -965,7 +999,10 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -983,7 +1020,10 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1001,7 +1041,10 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1019,7 +1062,10 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1037,7 +1083,10 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1055,7 +1104,10 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1073,7 +1125,10 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1091,7 +1146,10 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1109,7 +1167,10 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1127,7 +1188,10 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1145,7 +1209,10 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1163,7 +1230,10 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1"/>
+      <c r="A14" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1181,7 +1251,10 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1"/>
+      <c r="A15" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1199,7 +1272,10 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1"/>
+      <c r="A16" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1217,7 +1293,10 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1"/>
+      <c r="A17" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1242,13 +1321,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}">
-  <sheetPr codeName="Sheet2"/>
+  <sheetPr codeName="Sheet2" filterMode="1"/>
   <dimension ref="A1:AO45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E71" sqref="E71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1260,7 +1339,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>60</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1306,7 +1385,7 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1415,7 +1494,11 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1442,134 +1525,138 @@
       </c>
       <c r="J3" s="3">
         <f>'[2]links to constraints'!$C$4</f>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="K3" s="4">
         <f>J3</f>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="L3" s="4">
         <f t="shared" ref="L3:AO3" si="0">K3</f>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="M3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="N3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="O3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="P3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="Q3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="R3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="T3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="U3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="V3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="W3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="X3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="Y3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="Z3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AA3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AB3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AC3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AD3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AE3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AF3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AG3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AH3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AI3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AJ3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AK3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AL3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AM3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AN3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
+        <v>1.0643442529852023</v>
       </c>
       <c r="AO3" s="4">
         <f t="shared" si="0"/>
-        <v>1.6224025174380639</v>
-      </c>
-    </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+        <v>1.0643442529852023</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1691,7 +1778,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1813,7 +1904,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
@@ -1838,7 +1933,7 @@
       <c r="I6" s="1">
         <v>0</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="3">
         <f>'[2]links to constraints'!$C$5</f>
         <v>0.9305042796234908</v>
       </c>
@@ -1967,7 +2062,11 @@
         <v>0.9305042796234908</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2089,7 +2188,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
@@ -2211,7 +2314,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
@@ -2238,134 +2345,138 @@
       </c>
       <c r="J9" s="3">
         <f>'[2]links to constraints'!$C$6</f>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="K9" s="4">
         <f>J9</f>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="L9" s="4">
         <f t="shared" ref="L9:AO9" si="2">K9</f>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="M9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="N9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="O9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="P9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="S9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="T9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="U9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="V9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="W9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="X9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="Y9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="Z9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AA9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AB9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AC9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AD9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AE9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AF9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AG9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AH9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AI9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AJ9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AK9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AL9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AM9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AN9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
+        <v>0.2941969234853859</v>
       </c>
       <c r="AO9" s="4">
         <f t="shared" si="2"/>
-        <v>0.44845060979707235</v>
-      </c>
-    </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+        <v>0.2941969234853859</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -2487,7 +2598,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
@@ -2609,7 +2724,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
@@ -2634,7 +2753,7 @@
       <c r="I12" s="1">
         <v>0</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="3">
         <f>'[2]links to constraints'!$C$7</f>
         <v>3.0777317647058822</v>
       </c>
@@ -2763,7 +2882,11 @@
         <v>3.0777317647058822</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2885,7 +3008,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
@@ -3007,7 +3134,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
@@ -3032,136 +3163,140 @@
       <c r="I15" s="1">
         <v>0</v>
       </c>
-      <c r="J15" s="2">
+      <c r="J15" s="3">
         <f>'[2]links to constraints'!$C$8</f>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="K15" s="4">
         <f>J15</f>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="L15" s="4">
         <f t="shared" ref="L15:AO15" si="4">K15</f>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="M15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="N15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="O15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="P15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="S15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="T15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="U15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="V15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="W15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="X15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="Y15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="Z15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AA15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AB15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AC15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AD15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AE15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AF15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AG15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AH15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AI15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AJ15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AK15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AL15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AM15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AN15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
       <c r="AO15" s="4">
         <f t="shared" si="4"/>
-        <v>0.4152051071791632</v>
+        <v>1.719529411764706</v>
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
@@ -3283,7 +3418,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
@@ -3405,7 +3544,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -3527,7 +3670,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
@@ -3579,7 +3726,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="5">
         <f>-'[2]links to constraints'!$C$13</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
@@ -3587,7 +3734,7 @@
       <c r="AF19" s="2"/>
       <c r="AG19" s="2">
         <f>AB19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
@@ -3595,19 +3742,23 @@
       <c r="AK19" s="2"/>
       <c r="AL19" s="2">
         <f>AG19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2">
         <f>AL19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO19" s="2">
         <f>AN19</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="20" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
@@ -3729,7 +3880,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B21" s="1" t="s">
         <v>39</v>
       </c>
@@ -3791,7 +3946,11 @@
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
     </row>
-    <row r="22" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
@@ -3913,7 +4072,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B23" s="1" t="s">
         <v>39</v>
       </c>
@@ -3965,7 +4128,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2">
         <f>AB19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
@@ -3973,7 +4136,7 @@
       <c r="AF23" s="2"/>
       <c r="AG23" s="2">
         <f>AG19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
@@ -3981,19 +4144,23 @@
       <c r="AK23" s="2"/>
       <c r="AL23" s="2">
         <f>AL19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2">
         <f>AN19</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO23" s="2">
         <f>AO19</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="24" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B24" s="1" t="s">
         <v>39</v>
       </c>
@@ -4115,7 +4282,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
@@ -4177,7 +4348,11 @@
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
     </row>
-    <row r="26" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
@@ -4299,7 +4474,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
@@ -4351,7 +4530,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2">
         <f>AB23</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
@@ -4359,7 +4538,7 @@
       <c r="AF27" s="2"/>
       <c r="AG27" s="2">
         <f>AG23</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
@@ -4367,19 +4546,23 @@
       <c r="AK27" s="2"/>
       <c r="AL27" s="2">
         <f>AL23</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2">
         <f>AN23</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO27" s="2">
         <f>AO23</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="28" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
@@ -4501,7 +4684,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
@@ -4561,7 +4748,11 @@
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
     </row>
-    <row r="30" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
@@ -4683,7 +4874,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
@@ -4735,7 +4930,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2">
         <f>AB27</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
@@ -4743,7 +4938,7 @@
       <c r="AF31" s="2"/>
       <c r="AG31" s="2">
         <f>AG27</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
@@ -4751,19 +4946,23 @@
       <c r="AK31" s="2"/>
       <c r="AL31" s="2">
         <f>AL27</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2">
         <f>AN27</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO31" s="2">
         <f>AO27</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="32" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
@@ -4885,7 +5084,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B33" s="1" t="s">
         <v>39</v>
       </c>
@@ -4947,7 +5150,11 @@
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
     </row>
-    <row r="34" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
@@ -5069,7 +5276,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
@@ -5191,7 +5402,11 @@
         <v>-0.5</v>
       </c>
     </row>
-    <row r="36" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A36" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
@@ -5313,7 +5528,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
@@ -5365,7 +5584,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2">
         <f>AB31</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -5373,7 +5592,7 @@
       <c r="AF37" s="2"/>
       <c r="AG37" s="2">
         <f>AG31</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
@@ -5381,19 +5600,23 @@
       <c r="AK37" s="2"/>
       <c r="AL37" s="2">
         <f>AL31</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AM37" s="2"/>
       <c r="AN37" s="2">
         <f>AN31</f>
-        <v>-0.08</v>
+        <v>0.16</v>
       </c>
       <c r="AO37" s="2">
         <f>AO31</f>
-        <v>-0.08</v>
-      </c>
-    </row>
-    <row r="38" spans="2:41" x14ac:dyDescent="0.25">
+        <v>0.16</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B38" s="1" t="s">
         <v>39</v>
       </c>
@@ -5515,7 +5738,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
@@ -5575,7 +5802,11 @@
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
     </row>
-    <row r="40" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
@@ -5697,7 +5928,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B41" s="1" t="s">
         <v>59</v>
       </c>
@@ -5819,7 +6054,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B42" s="1" t="s">
         <v>59</v>
       </c>
@@ -5941,7 +6180,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B43" s="1" t="s">
         <v>59</v>
       </c>
@@ -6063,7 +6306,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B44" s="1" t="s">
         <v>59</v>
       </c>
@@ -6185,7 +6432,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="2:41" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B45" s="1" t="s">
         <v>59</v>
       </c>
@@ -6308,18 +6559,24 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO45" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}"/>
+  <autoFilter ref="A1:AO45" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="UC-IPPREC-MAX"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F99B7C9-5FBB-4C6F-BCA2-7100EC51A245}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6329,7 +6586,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
       <c r="B1" t="s">
@@ -6337,6 +6594,10 @@
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B2" s="1" t="s">
         <v>61</v>
       </c>
@@ -6363,6 +6624,10 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B3" s="1" t="s">
         <v>61</v>
       </c>
@@ -6389,6 +6654,10 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B4" s="1" t="s">
         <v>61</v>
       </c>
@@ -6415,6 +6684,10 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B5" s="1" t="s">
         <v>61</v>
       </c>
@@ -6441,6 +6714,10 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B6" s="1" t="s">
         <v>61</v>
       </c>
@@ -6467,6 +6744,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B7" s="1" t="s">
         <v>61</v>
       </c>
@@ -6493,6 +6774,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B8" s="1" t="s">
         <v>61</v>
       </c>
@@ -6519,6 +6804,10 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B9" s="1" t="s">
         <v>61</v>
       </c>
@@ -6545,6 +6834,10 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B10" s="1" t="s">
         <v>61</v>
       </c>
@@ -6571,6 +6864,10 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B11" s="1" t="s">
         <v>61</v>
       </c>
@@ -6597,6 +6894,10 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B12" s="1" t="s">
         <v>61</v>
       </c>
@@ -6623,6 +6924,10 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B13" s="1" t="s">
         <v>61</v>
       </c>
@@ -6649,6 +6954,10 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B14" s="1" t="s">
         <v>61</v>
       </c>
@@ -6675,6 +6984,10 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B15" s="1" t="s">
         <v>61</v>
       </c>
@@ -6701,6 +7014,10 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B16" s="1" t="s">
         <v>61</v>
       </c>
@@ -6726,7 +7043,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="str">
+        <f>IF(index!$B$2,"","*")</f>
+        <v>*</v>
+      </c>
       <c r="B17" s="1" t="s">
         <v>61</v>
       </c>

</xml_diff>

<commit_message>
Industry fixes and edits for REF industry - TCH_IND
Added biogas as alt fuel for NMM bricks (residual emissions) to BASE
Fixed major issue with clinker substitution - removed BF slag input to BFSLAG substitution causing it to run at BF's activity levels. 
new issue -- Chemical pulping in IPP has not enough capacity in BY, and is infeas without NCAP_START set to 2012 for -N tech. Not sure why this broke now.
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_IND/PP_constraints.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_IND/PP_constraints.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\TCH_IND\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC9D41A-85B3-4B13-8A4A-840DF547F435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADEEAA8F-68E0-4931-9DCD-9A32826671FA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E9085F61-4CF2-4A17-84B6-F025775E748A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E9085F61-4CF2-4A17-84B6-F025775E748A}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="63">
   <si>
     <t>REGION1</t>
   </si>
@@ -227,19 +227,10 @@
     <t>UCRULE_CAP</t>
   </si>
   <si>
-    <t>TS DATA</t>
-  </si>
-  <si>
     <t>UC_R_EACH</t>
   </si>
   <si>
-    <t>TID DATA</t>
-  </si>
-  <si>
     <t>*</t>
-  </si>
-  <si>
-    <t>ITEMS</t>
   </si>
   <si>
     <t>Import constraints to model?</t>
@@ -558,7 +549,7 @@
       <sheetData sheetId="3">
         <row r="2">
           <cell r="B2" t="b">
-            <v>1</v>
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -579,7 +570,7 @@
       <sheetData sheetId="18">
         <row r="1">
           <cell r="C1" t="b">
-            <v>0</v>
+            <v>1</v>
           </cell>
         </row>
         <row r="4">
@@ -609,7 +600,7 @@
         </row>
         <row r="13">
           <cell r="C13">
-            <v>-0.16</v>
+            <v>0</v>
           </cell>
         </row>
       </sheetData>
@@ -927,7 +918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04FDDD9F-2C3B-406C-A725-1972B126B5CE}">
   <dimension ref="B2:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -936,10 +927,10 @@
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="b">
         <f>'[2]links to constraints'!$C$1</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -953,7 +944,7 @@
   <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -966,8 +957,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>64</v>
+      <c r="A1" s="1" t="str">
+        <f>IF(index!$B$2,"ITEMS","")</f>
+        <v>ITEMS</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -978,10 +970,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -999,10 +988,6 @@
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
       <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
@@ -1020,10 +1005,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -1041,10 +1023,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -1062,10 +1041,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>1</v>
       </c>
@@ -1083,10 +1059,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>1</v>
       </c>
@@ -1104,10 +1077,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>1</v>
       </c>
@@ -1125,10 +1095,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>1</v>
       </c>
@@ -1146,10 +1113,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>1</v>
       </c>
@@ -1167,10 +1131,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>1</v>
       </c>
@@ -1188,10 +1149,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>1</v>
       </c>
@@ -1209,10 +1167,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>1</v>
       </c>
@@ -1230,10 +1185,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>1</v>
       </c>
@@ -1251,10 +1203,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>1</v>
       </c>
@@ -1272,10 +1221,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>1</v>
       </c>
@@ -1293,10 +1239,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>1</v>
       </c>
@@ -1323,11 +1266,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}">
-  <sheetPr codeName="Sheet2" filterMode="1"/>
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:AO45"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1339,8 +1282,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>60</v>
+      <c r="A1" s="1" t="str">
+        <f>IF(index!$B$2,"TS DATA","")</f>
+        <v>TS DATA</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1385,9 +1329,9 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
     </row>
-    <row r="2" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -1494,11 +1438,7 @@
         <v>2060</v>
       </c>
     </row>
-    <row r="3" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>36</v>
       </c>
@@ -1652,11 +1592,8 @@
         <v>1.0643442529852023</v>
       </c>
     </row>
-    <row r="4" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
@@ -1778,11 +1715,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>36</v>
       </c>
@@ -1904,11 +1838,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
         <v>36</v>
       </c>
@@ -2062,11 +1993,8 @@
         <v>0.9305042796234908</v>
       </c>
     </row>
-    <row r="7" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>36</v>
       </c>
@@ -2188,11 +2116,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>36</v>
       </c>
@@ -2314,11 +2239,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>36</v>
       </c>
@@ -2472,11 +2394,8 @@
         <v>0.2941969234853859</v>
       </c>
     </row>
-    <row r="10" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -2598,11 +2517,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>36</v>
       </c>
@@ -2724,11 +2640,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>36</v>
       </c>
@@ -2882,11 +2795,8 @@
         <v>3.0777317647058822</v>
       </c>
     </row>
-    <row r="13" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
@@ -3008,11 +2918,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>36</v>
       </c>
@@ -3134,11 +3041,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>36</v>
       </c>
@@ -3293,10 +3197,7 @@
       </c>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>36</v>
       </c>
@@ -3418,11 +3319,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>36</v>
       </c>
@@ -3544,11 +3442,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>36</v>
       </c>
@@ -3670,11 +3565,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>39</v>
       </c>
@@ -3698,7 +3590,7 @@
       </c>
       <c r="I19" s="1">
         <f>IF('[2]PAMS levers'!B$2,3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J19" s="1">
         <v>0</v>
@@ -3726,7 +3618,7 @@
       <c r="AA19" s="2"/>
       <c r="AB19" s="5">
         <f>-'[2]links to constraints'!$C$13</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="2"/>
       <c r="AD19" s="2"/>
@@ -3734,7 +3626,7 @@
       <c r="AF19" s="2"/>
       <c r="AG19" s="2">
         <f>AB19</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AH19" s="2"/>
       <c r="AI19" s="2"/>
@@ -3742,23 +3634,20 @@
       <c r="AK19" s="2"/>
       <c r="AL19" s="2">
         <f>AG19</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AM19" s="2"/>
       <c r="AN19" s="2">
         <f>AL19</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AO19" s="2">
         <f>AN19</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>39</v>
       </c>
@@ -3880,11 +3769,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>39</v>
       </c>
@@ -3946,11 +3832,8 @@
       <c r="AN21" s="1"/>
       <c r="AO21" s="1"/>
     </row>
-    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>39</v>
       </c>
@@ -4072,11 +3955,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>39</v>
       </c>
@@ -4100,7 +3980,7 @@
       </c>
       <c r="I23" s="1">
         <f>IF('[2]PAMS levers'!B$2,3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J23" s="1">
         <v>0</v>
@@ -4128,7 +4008,7 @@
       <c r="AA23" s="2"/>
       <c r="AB23" s="2">
         <f>AB19</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AC23" s="2"/>
       <c r="AD23" s="2"/>
@@ -4136,7 +4016,7 @@
       <c r="AF23" s="2"/>
       <c r="AG23" s="2">
         <f>AG19</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AH23" s="2"/>
       <c r="AI23" s="2"/>
@@ -4144,23 +4024,20 @@
       <c r="AK23" s="2"/>
       <c r="AL23" s="2">
         <f>AL19</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AM23" s="2"/>
       <c r="AN23" s="2">
         <f>AN19</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AO23" s="2">
         <f>AO19</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>39</v>
       </c>
@@ -4282,11 +4159,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>39</v>
       </c>
@@ -4348,11 +4222,8 @@
       <c r="AN25" s="1"/>
       <c r="AO25" s="1"/>
     </row>
-    <row r="26" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>39</v>
       </c>
@@ -4474,11 +4345,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
@@ -4502,7 +4370,7 @@
       </c>
       <c r="I27" s="1">
         <f>IF('[2]PAMS levers'!B$2,3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J27" s="1">
         <v>0</v>
@@ -4530,7 +4398,7 @@
       <c r="AA27" s="2"/>
       <c r="AB27" s="2">
         <f>AB23</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AC27" s="2"/>
       <c r="AD27" s="2"/>
@@ -4538,7 +4406,7 @@
       <c r="AF27" s="2"/>
       <c r="AG27" s="2">
         <f>AG23</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AH27" s="2"/>
       <c r="AI27" s="2"/>
@@ -4546,23 +4414,20 @@
       <c r="AK27" s="2"/>
       <c r="AL27" s="2">
         <f>AL23</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AM27" s="2"/>
       <c r="AN27" s="2">
         <f>AN23</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AO27" s="2">
         <f>AO23</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
       <c r="B28" s="1" t="s">
         <v>39</v>
       </c>
@@ -4684,11 +4549,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
       <c r="B29" s="1" t="s">
         <v>39</v>
       </c>
@@ -4748,11 +4610,8 @@
       <c r="AN29" s="1"/>
       <c r="AO29" s="1"/>
     </row>
-    <row r="30" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="30" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
       <c r="B30" s="1" t="s">
         <v>39</v>
       </c>
@@ -4874,11 +4733,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="31" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
       <c r="B31" s="1" t="s">
         <v>39</v>
       </c>
@@ -4902,7 +4758,7 @@
       </c>
       <c r="I31" s="1">
         <f>IF('[2]PAMS levers'!B$2,3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J31" s="1">
         <v>0</v>
@@ -4930,7 +4786,7 @@
       <c r="AA31" s="2"/>
       <c r="AB31" s="2">
         <f>AB27</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AC31" s="2"/>
       <c r="AD31" s="2"/>
@@ -4938,7 +4794,7 @@
       <c r="AF31" s="2"/>
       <c r="AG31" s="2">
         <f>AG27</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AH31" s="2"/>
       <c r="AI31" s="2"/>
@@ -4946,23 +4802,20 @@
       <c r="AK31" s="2"/>
       <c r="AL31" s="2">
         <f>AL27</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AM31" s="2"/>
       <c r="AN31" s="2">
         <f>AN27</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AO31" s="2">
         <f>AO27</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="32" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
       <c r="B32" s="1" t="s">
         <v>39</v>
       </c>
@@ -5084,11 +4937,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="33" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
       <c r="B33" s="1" t="s">
         <v>39</v>
       </c>
@@ -5150,11 +5000,8 @@
       <c r="AN33" s="1"/>
       <c r="AO33" s="1"/>
     </row>
-    <row r="34" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="34" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
       <c r="B34" s="1" t="s">
         <v>39</v>
       </c>
@@ -5277,10 +5124,7 @@
       </c>
     </row>
     <row r="35" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A35" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A35" s="1"/>
       <c r="B35" s="1" t="s">
         <v>39</v>
       </c>
@@ -5403,10 +5247,7 @@
       </c>
     </row>
     <row r="36" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A36" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A36" s="1"/>
       <c r="B36" s="1" t="s">
         <v>39</v>
       </c>
@@ -5528,11 +5369,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="37" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
       <c r="B37" s="1" t="s">
         <v>39</v>
       </c>
@@ -5556,7 +5394,7 @@
       </c>
       <c r="I37" s="1">
         <f>IF('[2]PAMS levers'!B$2,3,0)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="J37" s="1">
         <v>0</v>
@@ -5584,7 +5422,7 @@
       <c r="AA37" s="2"/>
       <c r="AB37" s="2">
         <f>AB31</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="2"/>
@@ -5592,7 +5430,7 @@
       <c r="AF37" s="2"/>
       <c r="AG37" s="2">
         <f>AG31</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AH37" s="2"/>
       <c r="AI37" s="2"/>
@@ -5600,23 +5438,20 @@
       <c r="AK37" s="2"/>
       <c r="AL37" s="2">
         <f>AL31</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AM37" s="2"/>
       <c r="AN37" s="2">
         <f>AN31</f>
-        <v>0.16</v>
+        <v>0</v>
       </c>
       <c r="AO37" s="2">
         <f>AO31</f>
-        <v>0.16</v>
-      </c>
-    </row>
-    <row r="38" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
       <c r="B38" s="1" t="s">
         <v>39</v>
       </c>
@@ -5738,11 +5573,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="39" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
       <c r="B39" s="1" t="s">
         <v>39</v>
       </c>
@@ -5802,11 +5634,8 @@
       <c r="AN39" s="1"/>
       <c r="AO39" s="1"/>
     </row>
-    <row r="40" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="40" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
       <c r="B40" s="1" t="s">
         <v>39</v>
       </c>
@@ -5928,11 +5757,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="41" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
       <c r="B41" s="1" t="s">
         <v>59</v>
       </c>
@@ -6054,11 +5880,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="42" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
       <c r="B42" s="1" t="s">
         <v>59</v>
       </c>
@@ -6180,11 +6003,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="43" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
       <c r="B43" s="1" t="s">
         <v>59</v>
       </c>
@@ -6306,11 +6126,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="44" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
       <c r="B44" s="1" t="s">
         <v>59</v>
       </c>
@@ -6432,11 +6249,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+    <row r="45" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
       <c r="B45" s="1" t="s">
         <v>59</v>
       </c>
@@ -6559,13 +6373,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AO45" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="UC-IPPREC-MAX"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:AO45" xr:uid="{477E96F8-3D3A-4EE1-82D3-E3DFF7E01791}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -6576,7 +6384,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6586,20 +6394,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>62</v>
+      <c r="A1" s="1" t="str">
+        <f>IF(index!$B$2,"TID DATA","")</f>
+        <v>TID DATA</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
@@ -6624,12 +6430,9 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -6654,12 +6457,9 @@
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>8</v>
@@ -6684,12 +6484,9 @@
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>10</v>
@@ -6714,12 +6511,9 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>12</v>
@@ -6744,12 +6538,9 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -6774,12 +6565,9 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -6804,12 +6592,9 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>18</v>
@@ -6834,12 +6619,9 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>20</v>
@@ -6864,12 +6646,9 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>22</v>
@@ -6894,12 +6673,9 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>24</v>
@@ -6924,12 +6700,9 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>26</v>
@@ -6954,12 +6727,9 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>28</v>
@@ -6984,12 +6754,9 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>30</v>
@@ -7014,12 +6781,9 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>32</v>
@@ -7044,12 +6808,9 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="str">
-        <f>IF(index!$B$2,"","*")</f>
-        <v>*</v>
-      </c>
+      <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>34</v>

</xml_diff>